<commit_message>
updates on metadata. creating EML
</commit_message>
<xml_diff>
--- a/4.project.115/Metadata.xlsx
+++ b/4.project.115/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargas/padl/pcarlson-chlorurus/4.project.115/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88F38C2-DF18-8F4E-9814-366A497997B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E2D227-1881-6F44-A188-055839195A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2203" uniqueCount="1205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="1206">
   <si>
     <t>csv_E</t>
   </si>
@@ -3882,9 +3882,6 @@
   </si>
   <si>
     <t>kud95_feeding_area</t>
-  </si>
-  <si>
-    <t>Species_full_name</t>
   </si>
   <si>
     <t>Location at which that individual fish was found</t>
@@ -4090,6 +4087,12 @@
   </si>
   <si>
     <t xml:space="preserve">Palmyra Atoll National Wildlife Refuge </t>
+  </si>
+  <si>
+    <t>PADL Data Manager</t>
+  </si>
+  <si>
+    <t>species_full_name</t>
   </si>
 </sst>
 </file>
@@ -4521,8 +4524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4578,7 +4581,7 @@
         <v>1083</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1084</v>
@@ -12828,7 +12831,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23:E28"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -12962,7 +12965,7 @@
         <v>1102</v>
       </c>
       <c r="D6" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E6" t="s">
         <v>1072</v>
@@ -13180,7 +13183,7 @@
         <v>1102</v>
       </c>
       <c r="D17" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E17" t="s">
         <v>1072</v>
@@ -13326,10 +13329,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>1136</v>
+        <v>1205</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>1072</v>
@@ -13346,7 +13349,7 @@
         <v>1099</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>1072</v>
@@ -13360,10 +13363,10 @@
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>1138</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>1139</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>1070</v>
@@ -13377,10 +13380,10 @@
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>1140</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>1141</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>1071</v>
@@ -13449,10 +13452,10 @@
         <v>1112</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E2" t="s">
         <v>1144</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1145</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -13466,10 +13469,10 @@
         <v>1112</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E3" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -13483,10 +13486,10 @@
         <v>1112</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E4" t="s">
         <v>1147</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1148</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -13503,7 +13506,7 @@
         <v>530</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -13517,10 +13520,10 @@
         <v>1112</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E6" t="s">
         <v>1150</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -13534,10 +13537,10 @@
         <v>1112</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E7" t="s">
         <v>1152</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1153</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -13551,10 +13554,10 @@
         <v>1112</v>
       </c>
       <c r="D8" s="14" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E8" t="s">
         <v>1154</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -13571,7 +13574,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -13585,10 +13588,10 @@
         <v>1112</v>
       </c>
       <c r="D10" s="14" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E10" t="s">
         <v>1157</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -13602,10 +13605,10 @@
         <v>1112</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E11" t="s">
         <v>1159</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -13619,10 +13622,10 @@
         <v>1074</v>
       </c>
       <c r="D12" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E12" t="s">
         <v>1162</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -13636,10 +13639,10 @@
         <v>1074</v>
       </c>
       <c r="D13" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E13" t="s">
         <v>1164</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1165</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -13653,10 +13656,10 @@
         <v>1074</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>1162</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -13670,10 +13673,10 @@
         <v>1074</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>1162</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -13687,10 +13690,10 @@
         <v>1074</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>1164</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>1165</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -13701,13 +13704,13 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D17" t="s">
+        <v>1165</v>
+      </c>
+      <c r="E17" t="s">
         <v>1166</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1167</v>
       </c>
     </row>
   </sheetData>
@@ -13757,7 +13760,7 @@
         <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -13768,7 +13771,7 @@
         <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -13779,7 +13782,7 @@
         <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -13796,7 +13799,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13832,7 +13835,7 @@
         <v>1076</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -13843,7 +13846,7 @@
         <v>1076</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1">
@@ -13854,7 +13857,7 @@
         <v>1076</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="1" customFormat="1">
@@ -13865,12 +13868,15 @@
         <v>1077</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>115</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1204</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1039</v>
@@ -13893,7 +13899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
@@ -13930,19 +13936,19 @@
         <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C2">
-        <v>5.8988500000000004</v>
+        <v>5.8833299999999999</v>
       </c>
       <c r="D2">
-        <v>5.85975</v>
+        <v>5.8710000000000004</v>
       </c>
       <c r="E2">
-        <v>-162.11319399999999</v>
+        <v>-162.04300000000001</v>
       </c>
       <c r="F2">
-        <v>-162.169399</v>
+        <v>-162.083</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1">
@@ -14251,14 +14257,14 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="10" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>1171</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>1172</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>1033</v>
@@ -14271,7 +14277,7 @@
       <c r="K10" s="18"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -14279,16 +14285,16 @@
     </row>
     <row r="11" spans="1:16" ht="16">
       <c r="A11" s="10" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>1175</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>1176</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>1147</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>1177</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>1033</v>
@@ -14301,26 +14307,26 @@
       <c r="K11" s="18"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="10" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>1179</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>1180</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>1033</v>
@@ -14333,7 +14339,7 @@
       <c r="K12" s="18"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -14341,14 +14347,14 @@
     </row>
     <row r="13" spans="1:16" ht="16">
       <c r="A13" s="10" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>1183</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>1184</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="19" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>1033</v>
@@ -14367,14 +14373,14 @@
     </row>
     <row r="14" spans="1:16" ht="16">
       <c r="A14" s="10" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>1186</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>1187</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="19" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>1033</v>
@@ -14393,14 +14399,14 @@
     </row>
     <row r="15" spans="1:16" ht="80">
       <c r="A15" s="10" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="19" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>1033</v>
@@ -14413,27 +14419,27 @@
       <c r="K15" s="18"/>
       <c r="L15" s="10"/>
       <c r="M15" s="4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="N15" s="20" t="s">
         <v>1196</v>
-      </c>
-      <c r="N15" s="20" t="s">
-        <v>1197</v>
       </c>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16" ht="16">
       <c r="A16" s="10" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>1190</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>1191</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="19" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>1192</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>1193</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="10"/>
@@ -14449,22 +14455,22 @@
     </row>
     <row r="17" spans="1:14" ht="16">
       <c r="A17" s="10" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>1198</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>1199</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>1200</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>1033</v>
       </c>
       <c r="M17" s="21" t="s">
+        <v>1200</v>
+      </c>
+      <c r="N17" s="22" t="s">
         <v>1201</v>
-      </c>
-      <c r="N17" s="22" t="s">
-        <v>1202</v>
       </c>
     </row>
   </sheetData>
@@ -14481,7 +14487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B25934-9280-524E-B624-293E63FB208B}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>